<commit_message>
de bugged delete API tests
</commit_message>
<xml_diff>
--- a/Manual_test_cases.xlsx
+++ b/Manual_test_cases.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.cariven\Documents\Backbase_Test_RC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.cariven\Documents\Computers_Database_Tests_RC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B33DE52-FDE1-4DDC-A951-2492301433AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA13FDE-D98E-4A3B-80F0-0F353595F49E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Tests" sheetId="1" r:id="rId1"/>
     <sheet name="Read and Update Tests" sheetId="2" r:id="rId2"/>
     <sheet name="Delete Tests" sheetId="3" r:id="rId3"/>
-    <sheet name="Issues" sheetId="4" r:id="rId4"/>
-    <sheet name="AP tests" sheetId="5" r:id="rId5"/>
+    <sheet name="API tests" sheetId="5" r:id="rId4"/>
+    <sheet name="Issues" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="227">
   <si>
     <t>Test Case</t>
   </si>
@@ -674,16 +674,239 @@
     <t>API Get Computers</t>
   </si>
   <si>
-    <t>Get computers</t>
-  </si>
-  <si>
     <t>at least 1 computer loaded into database</t>
   </si>
   <si>
-    <t>Postman GET http://computer-database.gatling.io/computers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List of computers </t>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>200 response, List of computers for first page</t>
+  </si>
+  <si>
+    <t>Using Postman send GET http://computer-database.gatling.io/computers</t>
+  </si>
+  <si>
+    <t>Using Postman send GET http://computer-database.gatling.io/computers?f=(test_computer_name)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">at least 2 computers loaded into database
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200 response 
+The filtered results are returned </t>
+  </si>
+  <si>
+    <t>API Get Filtered Computers</t>
+  </si>
+  <si>
+    <t>API Get Specific Computer</t>
+  </si>
+  <si>
+    <t>1 computer whos URL page is known</t>
+  </si>
+  <si>
+    <t>Using Postman send GET http://computer-database.gatling.io/computers/(computer url page number)</t>
+  </si>
+  <si>
+    <t>200 response 
+The specific computer is returned</t>
+  </si>
+  <si>
+    <t>API Create Computer</t>
+  </si>
+  <si>
+    <t>Using Postman send POST http://computer-database.gatling.io/computers/</t>
+  </si>
+  <si>
+    <t>200 response 
+The computer is created</t>
+  </si>
+  <si>
+    <t>{
+	"name" : "postman_Test_abc_edit",
+	"introduced" : "2000-01-01",
+	"discontinued" : "2000-01-", 
+	"company" : "3"	
+}</t>
+  </si>
+  <si>
+    <t>{
+	"name" : "",
+	"introduced" : "2000-01-01",
+	"discontinued" : "2000-01-", 
+	"company" : "3"	
+}</t>
+  </si>
+  <si>
+    <t>{
+	"name" : "",
+	"introduced" : "2000-01-01",
+	"discontinued" : "2000-01-", 
+	"company" : "99"	
+}</t>
+  </si>
+  <si>
+    <t>{
+	"name" : "",
+	"introduced" : "2000-01-01",
+	"discontinued" : "2000-01-", 
+	"company" : "a"	
+}</t>
+  </si>
+  <si>
+    <t>400 response the computer is not created</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>CD_Issues_07</t>
+  </si>
+  <si>
+    <t>API create Invalid Company</t>
+  </si>
+  <si>
+    <t>A computer with an unmapped comapany ID can be created</t>
+  </si>
+  <si>
+    <t>1). Using Postman send the Post Request {
+	"name" : "",
+	"introduced" : "2000-01-01",
+	"discontinued" : "2000-01-", 
+	"company" : "99"	
+}</t>
+  </si>
+  <si>
+    <t>As Company ID has not been mapped to an entry error should be returned</t>
+  </si>
+  <si>
+    <t>Computer is created, Company field in UI is empty</t>
+  </si>
+  <si>
+    <t>API Update Computer</t>
+  </si>
+  <si>
+    <t>{
+	"name" : "postman_Test_Create",
+	"introduced" : "2000-01-01",
+	"discontinued" : "2000-01-01", 
+	"company" : "3"	
+}</t>
+  </si>
+  <si>
+    <t>{
+	"name" : "postman_Test_Validation",
+	"introduced" : "2000-01-",
+	"discontinued" : "2000-01-01", 
+	"company" : "3"	
+}</t>
+  </si>
+  <si>
+    <t>Update details to.
+{
+	"name" : "postman_Update_Computer",
+	"introduced" : "2000-01-01",
+	"discontinued" : "2000-01-01", 
+	"company" : "3"	
+}</t>
+  </si>
+  <si>
+    <t>API Create Computer invalid intro date format</t>
+  </si>
+  <si>
+    <t>API Create Computer invalid disc date format</t>
+  </si>
+  <si>
+    <t>API Create Non Leap Year</t>
+  </si>
+  <si>
+    <t>{
+	"name" : "postman_Test_abc_edit",
+	"introduced" : "20-01-2001",
+	"discontinued" : "2001-02-29", 
+	"company" : "3"	
+}</t>
+  </si>
+  <si>
+    <t>Update details to.
+{
+	"name" : "postman_Update_Computer",
+	"introduced" : "2000-01-",
+	"discontinued" : "2000-01-01", 
+	"company" : "3"	
+}</t>
+  </si>
+  <si>
+    <t>API Update Computer Invalid intro Date</t>
+  </si>
+  <si>
+    <t>API Update Computer Invalid Discon Date</t>
+  </si>
+  <si>
+    <t>Update details to.
+{
+	"name" : "postman_Update_Computer",
+	"introduced" : "2000-01-01",
+	"discontinued" : "2000-01-", 
+	"company" : "3"	
+}</t>
+  </si>
+  <si>
+    <t>API Update Computer Invalid Date - non leap year</t>
+  </si>
+  <si>
+    <t>200 response 
+The computer is updated</t>
+  </si>
+  <si>
+    <t>400 Response the computer is not updated</t>
+  </si>
+  <si>
+    <t>API Update Computer Unmapped Company ID</t>
+  </si>
+  <si>
+    <t>Update details to.
+{
+	"name" : "postman_Update_Computer",
+	"introduced" : "2000-01-01",
+	"discontinued" : "2000-01-01", 
+	"company" : "99"	
+}</t>
+  </si>
+  <si>
+    <t>Update details to.
+{
+	"name" : "postman_Update_Computer",
+	"introduced" : "2000-01-01",
+	"discontinued" : "2000-01-01", 
+	"company" : "aa"	
+}</t>
+  </si>
+  <si>
+    <t>API Create Missing Name</t>
+  </si>
+  <si>
+    <t>API CreateUnmapped Company ID</t>
+  </si>
+  <si>
+    <t>API Create Invalid Company ID</t>
+  </si>
+  <si>
+    <t>API Update Invalid Company ID</t>
+  </si>
+  <si>
+    <t>Using Postman send POST http://computer-database.gatling.io/computers/computer to be updaetd url page number</t>
+  </si>
+  <si>
+    <t>API Delete Computer</t>
+  </si>
+  <si>
+    <t>Using Postman send POST http://computer-database.gatling.io/computers/computer to be updaetd url page number/delete</t>
+  </si>
+  <si>
+    <t>200 Response
+The computer is deleted</t>
   </si>
 </sst>
 </file>
@@ -896,130 +1119,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1434,482 +1666,482 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="66.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="91.28515625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="98.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="6" customWidth="1"/>
-    <col min="10" max="1026" width="11.5703125" style="6"/>
-    <col min="1027" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="8.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="91.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="98.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="5" customWidth="1"/>
+    <col min="10" max="1026" width="11.5703125" style="5"/>
+    <col min="1027" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="27" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24"/>
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:9" s="20" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="17"/>
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="19" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="7"/>
+      <c r="I2" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8">
+      <c r="A3" s="35"/>
+      <c r="B3" s="6">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="6" t="s">
+      <c r="H3" s="7"/>
+      <c r="I3" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8">
+      <c r="A4" s="35"/>
+      <c r="B4" s="6">
         <v>3</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8">
+      <c r="A5" s="35"/>
+      <c r="B5" s="6">
         <v>4</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="6" t="s">
+      <c r="H5" s="8"/>
+      <c r="I5" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8">
+      <c r="A6" s="35"/>
+      <c r="B6" s="6">
         <v>5</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="6" t="s">
+      <c r="H6" s="8"/>
+      <c r="I6" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8">
+      <c r="A7" s="35"/>
+      <c r="B7" s="6">
         <v>8</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="6" t="s">
+      <c r="H7" s="7"/>
+      <c r="I7" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8">
+      <c r="A8" s="35"/>
+      <c r="B8" s="6">
         <v>9</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="6" t="s">
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="6" t="s">
+      <c r="H8" s="7"/>
+      <c r="I8" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8">
+      <c r="A9" s="35"/>
+      <c r="B9" s="6">
         <v>10</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="6" t="s">
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="6" t="s">
+      <c r="H9" s="7"/>
+      <c r="I9" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8" t="s">
+      <c r="A10" s="35"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="6" t="s">
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="6" t="s">
+      <c r="H10" s="7"/>
+      <c r="I10" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8">
+      <c r="A11" s="35"/>
+      <c r="B11" s="6">
         <v>11</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>124</v>
       </c>
       <c r="H11" t="s">
         <v>113</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8">
+      <c r="A12" s="35"/>
+      <c r="B12" s="6">
         <v>12</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="11" t="s">
+      <c r="E12" s="36"/>
+      <c r="F12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>124</v>
       </c>
       <c r="H12" t="s">
         <v>121</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8">
+      <c r="A13" s="35"/>
+      <c r="B13" s="6">
         <v>13</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1" t="s">
+      <c r="E13" s="36"/>
+      <c r="F13" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="6" t="s">
+      <c r="H13" s="7"/>
+      <c r="I13" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8">
+      <c r="A14" s="35"/>
+      <c r="B14" s="6">
         <v>14</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="6" t="s">
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="6" t="s">
+      <c r="H14" s="7"/>
+      <c r="I14" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8">
+      <c r="A15" s="35"/>
+      <c r="B15" s="6">
         <v>15</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="6" t="s">
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="6" t="s">
+      <c r="H15" s="7"/>
+      <c r="I15" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8">
+      <c r="A16" s="35"/>
+      <c r="B16" s="6">
         <v>16</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="6" t="s">
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="6" t="s">
+      <c r="H16" s="7"/>
+      <c r="I16" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8">
+      <c r="A17" s="35"/>
+      <c r="B17" s="6">
         <v>17</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="6" t="s">
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="6" t="s">
+      <c r="H17" s="7"/>
+      <c r="I17" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8">
+      <c r="A18" s="35"/>
+      <c r="B18" s="6">
         <v>18</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="6" t="s">
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="6" t="s">
+      <c r="H18" s="7"/>
+      <c r="I18" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8">
+      <c r="A19" s="35"/>
+      <c r="B19" s="6">
         <v>19</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="6" t="s">
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="6" t="s">
+      <c r="H19" s="7"/>
+      <c r="I19" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8">
+      <c r="A20" s="35"/>
+      <c r="B20" s="6">
         <v>23</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="2" t="s">
+      <c r="D20" s="6"/>
+      <c r="E20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="5" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1940,429 +2172,429 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="34" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.7109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="45.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="34" style="6"/>
+    <col min="1" max="1" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="45.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="34" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="36" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="130.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="6">
         <v>26</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="211.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
-      <c r="B3" s="11">
+      <c r="A3" s="39"/>
+      <c r="B3" s="9">
         <v>27</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="6" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
-      <c r="B4" s="11">
+      <c r="A4" s="39"/>
+      <c r="B4" s="9">
         <v>29</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="H4" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="6" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
-      <c r="B5" s="11">
+      <c r="A5" s="39"/>
+      <c r="B5" s="9">
         <v>30</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="6" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
-      <c r="B6" s="8">
+      <c r="A6" s="39"/>
+      <c r="B6" s="6">
         <v>31</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="8" t="s">
+      <c r="F6" s="1"/>
+      <c r="G6" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="6" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="8">
+      <c r="A7" s="39"/>
+      <c r="B7" s="6">
         <v>32</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8" t="s">
+      <c r="H7" s="6"/>
+      <c r="I7" s="6" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
-      <c r="B8" s="8">
+      <c r="A8" s="39"/>
+      <c r="B8" s="6">
         <v>33</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="6"/>
+      <c r="E8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8" t="s">
+      <c r="H8" s="6"/>
+      <c r="I8" s="6" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
-      <c r="B9" s="21">
+      <c r="A9" s="39"/>
+      <c r="B9" s="14">
         <v>34</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8" t="s">
+      <c r="H9" s="6"/>
+      <c r="I9" s="6" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="22" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8" t="s">
+      <c r="H10" s="6"/>
+      <c r="I10" s="6" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <v>35</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="36"/>
+      <c r="E11" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8" t="s">
+      <c r="H11" s="6"/>
+      <c r="I11" s="6" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="29"/>
-      <c r="B12" s="8">
+      <c r="A12" s="38"/>
+      <c r="B12" s="6">
         <v>36</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2" t="s">
+      <c r="D12" s="36"/>
+      <c r="E12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8" t="s">
+      <c r="H12" s="6"/>
+      <c r="I12" s="6" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A13" s="29"/>
-      <c r="B13" s="8">
+      <c r="A13" s="38"/>
+      <c r="B13" s="6">
         <v>37</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2" t="s">
+      <c r="D13" s="36"/>
+      <c r="E13" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="H13" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="6" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="29"/>
-      <c r="B14" s="8">
+      <c r="A14" s="38"/>
+      <c r="B14" s="6">
         <v>38</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="2" t="s">
+      <c r="D14" s="36"/>
+      <c r="E14" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8" t="s">
+      <c r="H14" s="6"/>
+      <c r="I14" s="6" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="29"/>
-      <c r="B15" s="8">
+      <c r="A15" s="38"/>
+      <c r="B15" s="6">
         <v>39</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2" t="s">
+      <c r="D15" s="36"/>
+      <c r="E15" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8" t="s">
+      <c r="H15" s="6"/>
+      <c r="I15" s="6" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="29"/>
-      <c r="B16" s="30">
+      <c r="A16" s="38"/>
+      <c r="B16" s="21">
         <v>40</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8" t="s">
+      <c r="H16" s="6"/>
+      <c r="I16" s="6" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="29"/>
-      <c r="B17" s="8">
+      <c r="A17" s="38"/>
+      <c r="B17" s="6">
         <v>41</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8" t="s">
+      <c r="H17" s="6"/>
+      <c r="I17" s="6" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2380,167 +2612,167 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D50C73-AC1A-4B4D-ADA9-A016DC2EB872}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.7109375" defaultRowHeight="136.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="52.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="40.7109375" style="13"/>
+    <col min="1" max="1" width="6.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="40.7109375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="35"/>
-      <c r="B1" s="36" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="25" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="136.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="35"/>
-      <c r="B2" s="33">
+      <c r="A2" s="26"/>
+      <c r="B2" s="24">
         <v>41</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="10" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="136.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="33">
+      <c r="B3" s="24">
         <v>42</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="10" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="192" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="37"/>
-      <c r="B4" s="33">
+      <c r="A4" s="40"/>
+      <c r="B4" s="24">
         <v>43</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="10" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="136.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="37"/>
-      <c r="B5" s="33">
+      <c r="A5" s="40"/>
+      <c r="B5" s="24">
         <v>44</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="28" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="222.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="13">
+      <c r="B6" s="10">
         <v>45</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="28" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2553,194 +2785,830 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE706DD-C5DD-4F14-BE9A-3C2E4DB87D0F}">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6B6D70-9297-4BA7-AA2E-4B3FD3283A7E}">
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="37.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.42578125" style="10"/>
+    <col min="2" max="2" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="21" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="37.42578125" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="30"/>
+      <c r="B1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="24">
+        <v>46</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="43"/>
+      <c r="B3" s="24">
+        <v>47</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="44"/>
+      <c r="B4" s="24">
+        <v>48</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="24">
+        <v>49</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="43"/>
+      <c r="B6" s="24">
+        <v>50</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>193</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="43"/>
+      <c r="B7" s="24">
+        <v>51</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="F7" s="43"/>
+      <c r="G7" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="43"/>
+      <c r="B8" s="24">
+        <v>52</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="F8" s="43"/>
+      <c r="G8" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="43"/>
+      <c r="B9" s="24">
+        <v>53</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="F9" s="43"/>
+      <c r="G9" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="43"/>
+      <c r="B10" s="23">
+        <v>54</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="F10" s="43"/>
+      <c r="G10" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="44"/>
+      <c r="B11" s="24">
+        <v>55</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="F11" s="44"/>
+      <c r="G11" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A12" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="24">
+        <v>56</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="43"/>
+      <c r="B13" s="24">
+        <v>57</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A14" s="43"/>
+      <c r="B14" s="24">
+        <v>58</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="F14" s="43"/>
+      <c r="G14" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="43"/>
+      <c r="B15" s="24">
+        <v>59</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="F15" s="43"/>
+      <c r="G15" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A16" s="43"/>
+      <c r="B16" s="24">
+        <v>60</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="F16" s="43"/>
+      <c r="G16" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A17" s="44"/>
+      <c r="B17" s="24">
+        <v>61</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="F17" s="44"/>
+      <c r="G17" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="24">
+        <v>62</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="24"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="F6:F11"/>
+    <mergeCell ref="F13:F17"/>
+    <mergeCell ref="A12:A17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE706DD-C5DD-4F14-BE9A-3C2E4DB87D0F}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="44.5703125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="13" customWidth="1"/>
-    <col min="7" max="7" width="27" style="13" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="15.28515625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="27" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
     </row>
     <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="24" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="24" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="24" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="G6" s="24" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="G7" s="24" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="G8" s="33" t="s">
+      <c r="G8" s="24" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="G9" s="24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="G10" s="24" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2750,389 +3618,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6B6D70-9297-4BA7-AA2E-4B3FD3283A7E}">
-  <dimension ref="A1:I30"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="37.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="37.42578125" style="13"/>
-    <col min="2" max="2" width="14.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="37.42578125" style="13"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="54" x14ac:dyDescent="0.2">
-      <c r="A1" s="40"/>
-      <c r="B1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>176</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="33"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="33"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="33"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="33"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="33"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="33"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="33"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="33"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="33"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="33"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="33"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>